<commit_message>
bug fixed when app started
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11300" yWindow="2540" windowWidth="15520" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="10080" yWindow="2540" windowWidth="15520" windowHeight="11160" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="student-schema" sheetId="1" r:id="rId1"/>
     <sheet name="course-schema" sheetId="2" r:id="rId2"/>
     <sheet name="course-pseudodatac" sheetId="5" r:id="rId3"/>
     <sheet name="attendance-schema" sheetId="4" r:id="rId4"/>
+    <sheet name="instructor-schema" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
   <si>
     <t>Field Name</t>
   </si>
@@ -189,6 +190,9 @@
   </si>
   <si>
     <t>^Fri</t>
+  </si>
+  <si>
+    <t>instructor_id</t>
   </si>
 </sst>
 </file>
@@ -516,7 +520,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="A5:D7"/>
+      <selection activeCell="E7" sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -677,10 +681,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,7 +694,7 @@
     <col min="5" max="5" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -713,8 +717,11 @@
         <v>30</v>
       </c>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -730,8 +737,11 @@
       <c r="H2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -747,8 +757,11 @@
       <c r="H3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -764,8 +777,11 @@
       <c r="H4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -781,8 +797,11 @@
       <c r="H5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -798,8 +817,11 @@
       <c r="H6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -815,8 +837,11 @@
       <c r="H7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -832,8 +857,11 @@
       <c r="H8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -849,8 +877,11 @@
       <c r="H9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -866,8 +897,11 @@
       <c r="H10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -882,6 +916,9 @@
       </c>
       <c r="H11" t="s">
         <v>52</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -984,4 +1021,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="L1:P4"/>
+  <sheetViews>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="12:16" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="12:16" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="12:16" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="12:16" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>